<commit_message>
update with latest data
</commit_message>
<xml_diff>
--- a/outputs/concern_classification.xlsx
+++ b/outputs/concern_classification.xlsx
@@ -6117,7 +6117,7 @@
         <v>0.25</v>
       </c>
       <c r="H134">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I134">
         <v>5</v>
@@ -6160,7 +6160,7 @@
         <v>0.25</v>
       </c>
       <c r="H135">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I135">
         <v>5</v>
@@ -6203,7 +6203,7 @@
         <v>0.25</v>
       </c>
       <c r="H136">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I136">
         <v>5</v>
@@ -6246,7 +6246,7 @@
         <v>0.25</v>
       </c>
       <c r="H137">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I137">
         <v>5</v>
@@ -6332,7 +6332,7 @@
         <v>0.25</v>
       </c>
       <c r="H139">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I139">
         <v>5</v>
@@ -6461,7 +6461,7 @@
         <v>0.25</v>
       </c>
       <c r="H142">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I142">
         <v>5</v>
@@ -6504,7 +6504,7 @@
         <v>0.25</v>
       </c>
       <c r="H143">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I143">
         <v>5</v>
@@ -6547,7 +6547,7 @@
         <v>0.25</v>
       </c>
       <c r="H144">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I144">
         <v>5</v>
@@ -6590,7 +6590,7 @@
         <v>0.25</v>
       </c>
       <c r="H145">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I145">
         <v>5</v>
@@ -8138,7 +8138,7 @@
         <v>0.29</v>
       </c>
       <c r="H181">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I181">
         <v>4</v>
@@ -9865,7 +9865,7 @@
       </c>
       <c r="J221" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="K221" t="inlineStr">
@@ -9994,7 +9994,7 @@
       </c>
       <c r="J224" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>HIGH</t>
         </is>
       </c>
       <c r="K224" t="inlineStr">
@@ -10338,7 +10338,7 @@
       </c>
       <c r="J232" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>MID</t>
         </is>
       </c>
       <c r="K232" t="inlineStr">
@@ -10682,7 +10682,7 @@
       </c>
       <c r="J240" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>MID</t>
         </is>
       </c>
       <c r="K240" t="inlineStr">
@@ -10940,7 +10940,7 @@
       </c>
       <c r="J246" t="inlineStr">
         <is>
-          <t>HIGH</t>
+          <t>MID</t>
         </is>
       </c>
       <c r="K246" t="inlineStr">
@@ -12094,7 +12094,7 @@
         <v>0.36</v>
       </c>
       <c r="H273">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I273">
         <v>4</v>
@@ -12223,7 +12223,7 @@
         <v>0.37</v>
       </c>
       <c r="H276">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I276">
         <v>4</v>
@@ -12395,7 +12395,7 @@
         <v>0.37</v>
       </c>
       <c r="H280">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I280">
         <v>4</v>
@@ -12438,7 +12438,7 @@
         <v>0.37</v>
       </c>
       <c r="H281">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I281">
         <v>4</v>
@@ -12653,7 +12653,7 @@
         <v>0.38</v>
       </c>
       <c r="H286">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I286">
         <v>3</v>
@@ -12954,7 +12954,7 @@
         <v>0.38</v>
       </c>
       <c r="H293">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I293">
         <v>3</v>
@@ -19060,7 +19060,7 @@
         <v>0.48</v>
       </c>
       <c r="H435">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I435">
         <v>3</v>
@@ -19189,7 +19189,7 @@
         <v>0.49</v>
       </c>
       <c r="H438">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I438">
         <v>2</v>
@@ -19318,7 +19318,7 @@
         <v>0.49</v>
       </c>
       <c r="H441">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I441">
         <v>2</v>
@@ -19361,7 +19361,7 @@
         <v>0.49</v>
       </c>
       <c r="H442">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I442">
         <v>2</v>
@@ -19619,7 +19619,7 @@
         <v>0.49</v>
       </c>
       <c r="H448">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I448">
         <v>2</v>
@@ -20307,7 +20307,7 @@
         <v>0.5</v>
       </c>
       <c r="H464">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I464">
         <v>2</v>
@@ -21475,7 +21475,7 @@
       </c>
       <c r="J491" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
       <c r="K491" t="inlineStr">
@@ -21561,7 +21561,7 @@
       </c>
       <c r="J493" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
       <c r="K493" t="inlineStr">
@@ -25381,7 +25381,7 @@
         <v>0.59</v>
       </c>
       <c r="H582">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I582">
         <v>2</v>
@@ -25682,7 +25682,7 @@
         <v>0.6</v>
       </c>
       <c r="H589">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I589">
         <v>1</v>
@@ -25768,7 +25768,7 @@
         <v>0.6</v>
       </c>
       <c r="H591">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I591">
         <v>1</v>
@@ -25940,7 +25940,7 @@
         <v>0.6</v>
       </c>
       <c r="H595">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I595">
         <v>1</v>
@@ -30326,9 +30326,17 @@
       <c r="G697">
         <v>0.74</v>
       </c>
+      <c r="H697">
+        <v>1</v>
+      </c>
       <c r="I697">
         <v>1</v>
       </c>
+      <c r="J697" t="inlineStr">
+        <is>
+          <t>LOW</t>
+        </is>
+      </c>
       <c r="K697" t="inlineStr">
         <is>
           <t>LOW</t>
@@ -30404,9 +30412,17 @@
       <c r="G699">
         <v>0.74</v>
       </c>
+      <c r="H699">
+        <v>1</v>
+      </c>
       <c r="I699">
         <v>1</v>
       </c>
+      <c r="J699" t="inlineStr">
+        <is>
+          <t>LOW</t>
+        </is>
+      </c>
       <c r="K699" t="inlineStr">
         <is>
           <t>LOW</t>
@@ -30492,14 +30508,6 @@
       </c>
       <c r="G702">
         <v>0.75</v>
-      </c>
-      <c r="H702">
-        <v>1</v>
-      </c>
-      <c r="J702" t="inlineStr">
-        <is>
-          <t>LOW</t>
-        </is>
       </c>
     </row>
     <row r="703">

</xml_diff>

<commit_message>
debugging summaries+plotting and recreating plot1
</commit_message>
<xml_diff>
--- a/outputs/concern_classification.xlsx
+++ b/outputs/concern_classification.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K737"/>
+  <dimension ref="A1:K699"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6120,7 +6120,7 @@
         <v>5</v>
       </c>
       <c r="I134">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J134" t="inlineStr">
         <is>
@@ -6163,7 +6163,7 @@
         <v>5</v>
       </c>
       <c r="I135">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J135" t="inlineStr">
         <is>
@@ -6206,7 +6206,7 @@
         <v>5</v>
       </c>
       <c r="I136">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J136" t="inlineStr">
         <is>
@@ -6249,7 +6249,7 @@
         <v>5</v>
       </c>
       <c r="I137">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J137" t="inlineStr">
         <is>
@@ -6292,7 +6292,7 @@
         <v>5</v>
       </c>
       <c r="I138">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J138" t="inlineStr">
         <is>
@@ -6335,7 +6335,7 @@
         <v>5</v>
       </c>
       <c r="I139">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J139" t="inlineStr">
         <is>
@@ -6378,7 +6378,7 @@
         <v>5</v>
       </c>
       <c r="I140">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J140" t="inlineStr">
         <is>
@@ -6421,7 +6421,7 @@
         <v>5</v>
       </c>
       <c r="I141">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J141" t="inlineStr">
         <is>
@@ -6464,7 +6464,7 @@
         <v>5</v>
       </c>
       <c r="I142">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J142" t="inlineStr">
         <is>
@@ -6507,7 +6507,7 @@
         <v>5</v>
       </c>
       <c r="I143">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J143" t="inlineStr">
         <is>
@@ -6550,7 +6550,7 @@
         <v>5</v>
       </c>
       <c r="I144">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J144" t="inlineStr">
         <is>
@@ -6593,7 +6593,7 @@
         <v>5</v>
       </c>
       <c r="I145">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="J145" t="inlineStr">
         <is>
@@ -12183,7 +12183,7 @@
         <v>4</v>
       </c>
       <c r="I275">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J275" t="inlineStr">
         <is>
@@ -12226,7 +12226,7 @@
         <v>4</v>
       </c>
       <c r="I276">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J276" t="inlineStr">
         <is>
@@ -12269,7 +12269,7 @@
         <v>4</v>
       </c>
       <c r="I277">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J277" t="inlineStr">
         <is>
@@ -12312,7 +12312,7 @@
         <v>4</v>
       </c>
       <c r="I278">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J278" t="inlineStr">
         <is>
@@ -12355,7 +12355,7 @@
         <v>4</v>
       </c>
       <c r="I279">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J279" t="inlineStr">
         <is>
@@ -12398,7 +12398,7 @@
         <v>4</v>
       </c>
       <c r="I280">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J280" t="inlineStr">
         <is>
@@ -12441,7 +12441,7 @@
         <v>4</v>
       </c>
       <c r="I281">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J281" t="inlineStr">
         <is>
@@ -18246,7 +18246,7 @@
         <v>3</v>
       </c>
       <c r="I416">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J416" t="inlineStr">
         <is>
@@ -18289,7 +18289,7 @@
         <v>3</v>
       </c>
       <c r="I417">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J417" t="inlineStr">
         <is>
@@ -18332,7 +18332,7 @@
         <v>3</v>
       </c>
       <c r="I418">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J418" t="inlineStr">
         <is>
@@ -18375,7 +18375,7 @@
         <v>3</v>
       </c>
       <c r="I419">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J419" t="inlineStr">
         <is>
@@ -18418,7 +18418,7 @@
         <v>3</v>
       </c>
       <c r="I420">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J420" t="inlineStr">
         <is>
@@ -18461,7 +18461,7 @@
         <v>3</v>
       </c>
       <c r="I421">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J421" t="inlineStr">
         <is>
@@ -18504,7 +18504,7 @@
         <v>3</v>
       </c>
       <c r="I422">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J422" t="inlineStr">
         <is>
@@ -18547,7 +18547,7 @@
         <v>3</v>
       </c>
       <c r="I423">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J423" t="inlineStr">
         <is>
@@ -18590,7 +18590,7 @@
         <v>3</v>
       </c>
       <c r="I424">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J424" t="inlineStr">
         <is>
@@ -18633,7 +18633,7 @@
         <v>3</v>
       </c>
       <c r="I425">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J425" t="inlineStr">
         <is>
@@ -18676,7 +18676,7 @@
         <v>3</v>
       </c>
       <c r="I426">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J426" t="inlineStr">
         <is>
@@ -18719,7 +18719,7 @@
         <v>3</v>
       </c>
       <c r="I427">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J427" t="inlineStr">
         <is>
@@ -18762,7 +18762,7 @@
         <v>3</v>
       </c>
       <c r="I428">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J428" t="inlineStr">
         <is>
@@ -18805,7 +18805,7 @@
         <v>3</v>
       </c>
       <c r="I429">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J429" t="inlineStr">
         <is>
@@ -18848,7 +18848,7 @@
         <v>3</v>
       </c>
       <c r="I430">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J430" t="inlineStr">
         <is>
@@ -18891,7 +18891,7 @@
         <v>3</v>
       </c>
       <c r="I431">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J431" t="inlineStr">
         <is>
@@ -18934,7 +18934,7 @@
         <v>3</v>
       </c>
       <c r="I432">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J432" t="inlineStr">
         <is>
@@ -18977,7 +18977,7 @@
         <v>3</v>
       </c>
       <c r="I433">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J433" t="inlineStr">
         <is>
@@ -19020,7 +19020,7 @@
         <v>3</v>
       </c>
       <c r="I434">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J434" t="inlineStr">
         <is>
@@ -19063,7 +19063,7 @@
         <v>3</v>
       </c>
       <c r="I435">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J435" t="inlineStr">
         <is>
@@ -19846,7 +19846,7 @@
       </c>
       <c r="K453" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
     </row>
@@ -19889,7 +19889,7 @@
       </c>
       <c r="K454" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
     </row>
@@ -19932,7 +19932,7 @@
       </c>
       <c r="K455" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
     </row>
@@ -19975,7 +19975,7 @@
       </c>
       <c r="K456" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
     </row>
@@ -20018,7 +20018,7 @@
       </c>
       <c r="K457" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
     </row>
@@ -20061,7 +20061,7 @@
       </c>
       <c r="K458" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
     </row>
@@ -20104,7 +20104,7 @@
       </c>
       <c r="K459" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
     </row>
@@ -20147,7 +20147,7 @@
       </c>
       <c r="K460" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
     </row>
@@ -20190,7 +20190,7 @@
       </c>
       <c r="K461" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
     </row>
@@ -20233,7 +20233,7 @@
       </c>
       <c r="K462" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
     </row>
@@ -20276,7 +20276,7 @@
       </c>
       <c r="K463" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
     </row>
@@ -20319,7 +20319,7 @@
       </c>
       <c r="K464" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
     </row>
@@ -20362,7 +20362,7 @@
       </c>
       <c r="K465" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
     </row>
@@ -20405,7 +20405,7 @@
       </c>
       <c r="K466" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
     </row>
@@ -20448,7 +20448,7 @@
       </c>
       <c r="K467" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
     </row>
@@ -20491,7 +20491,7 @@
       </c>
       <c r="K468" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
     </row>
@@ -20534,7 +20534,7 @@
       </c>
       <c r="K469" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
     </row>
@@ -20577,7 +20577,7 @@
       </c>
       <c r="K470" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
     </row>
@@ -20620,7 +20620,7 @@
       </c>
       <c r="K471" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
     </row>
@@ -20663,7 +20663,7 @@
       </c>
       <c r="K472" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
     </row>
@@ -20706,7 +20706,7 @@
       </c>
       <c r="K473" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
     </row>
@@ -20749,7 +20749,7 @@
       </c>
       <c r="K474" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
     </row>
@@ -20792,7 +20792,7 @@
       </c>
       <c r="K475" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
     </row>
@@ -20835,7 +20835,7 @@
       </c>
       <c r="K476" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
     </row>
@@ -20878,7 +20878,7 @@
       </c>
       <c r="K477" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
     </row>
@@ -20921,7 +20921,7 @@
       </c>
       <c r="K478" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
     </row>
@@ -20964,7 +20964,7 @@
       </c>
       <c r="K479" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
     </row>
@@ -21007,7 +21007,7 @@
       </c>
       <c r="K480" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
     </row>
@@ -21050,7 +21050,7 @@
       </c>
       <c r="K481" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
     </row>
@@ -21093,7 +21093,7 @@
       </c>
       <c r="K482" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
     </row>
@@ -21136,7 +21136,7 @@
       </c>
       <c r="K483" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
     </row>
@@ -21179,7 +21179,7 @@
       </c>
       <c r="K484" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
     </row>
@@ -21222,7 +21222,7 @@
       </c>
       <c r="K485" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
     </row>
@@ -21265,7 +21265,7 @@
       </c>
       <c r="K486" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
     </row>
@@ -21308,7 +21308,7 @@
       </c>
       <c r="K487" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
     </row>
@@ -21351,7 +21351,7 @@
       </c>
       <c r="K488" t="inlineStr">
         <is>
-          <t>MID</t>
+          <t>LOW</t>
         </is>
       </c>
     </row>
@@ -24051,7 +24051,7 @@
         <v>2</v>
       </c>
       <c r="I551">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J551" t="inlineStr">
         <is>
@@ -24094,7 +24094,7 @@
         <v>2</v>
       </c>
       <c r="I552">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J552" t="inlineStr">
         <is>
@@ -24137,7 +24137,7 @@
         <v>2</v>
       </c>
       <c r="I553">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J553" t="inlineStr">
         <is>
@@ -24180,7 +24180,7 @@
         <v>2</v>
       </c>
       <c r="I554">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J554" t="inlineStr">
         <is>
@@ -24223,7 +24223,7 @@
         <v>2</v>
       </c>
       <c r="I555">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J555" t="inlineStr">
         <is>
@@ -24266,7 +24266,7 @@
         <v>2</v>
       </c>
       <c r="I556">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J556" t="inlineStr">
         <is>
@@ -24309,7 +24309,7 @@
         <v>2</v>
       </c>
       <c r="I557">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J557" t="inlineStr">
         <is>
@@ -24352,7 +24352,7 @@
         <v>2</v>
       </c>
       <c r="I558">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J558" t="inlineStr">
         <is>
@@ -24395,7 +24395,7 @@
         <v>2</v>
       </c>
       <c r="I559">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J559" t="inlineStr">
         <is>
@@ -24438,7 +24438,7 @@
         <v>2</v>
       </c>
       <c r="I560">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J560" t="inlineStr">
         <is>
@@ -24481,7 +24481,7 @@
         <v>2</v>
       </c>
       <c r="I561">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J561" t="inlineStr">
         <is>
@@ -24524,7 +24524,7 @@
         <v>2</v>
       </c>
       <c r="I562">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J562" t="inlineStr">
         <is>
@@ -24567,7 +24567,7 @@
         <v>2</v>
       </c>
       <c r="I563">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J563" t="inlineStr">
         <is>
@@ -24610,7 +24610,7 @@
         <v>2</v>
       </c>
       <c r="I564">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J564" t="inlineStr">
         <is>
@@ -24653,7 +24653,7 @@
         <v>2</v>
       </c>
       <c r="I565">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J565" t="inlineStr">
         <is>
@@ -24696,7 +24696,7 @@
         <v>2</v>
       </c>
       <c r="I566">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J566" t="inlineStr">
         <is>
@@ -24739,7 +24739,7 @@
         <v>2</v>
       </c>
       <c r="I567">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J567" t="inlineStr">
         <is>
@@ -24782,7 +24782,7 @@
         <v>2</v>
       </c>
       <c r="I568">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J568" t="inlineStr">
         <is>
@@ -24825,7 +24825,7 @@
         <v>2</v>
       </c>
       <c r="I569">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J569" t="inlineStr">
         <is>
@@ -24868,7 +24868,7 @@
         <v>2</v>
       </c>
       <c r="I570">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J570" t="inlineStr">
         <is>
@@ -24911,7 +24911,7 @@
         <v>2</v>
       </c>
       <c r="I571">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J571" t="inlineStr">
         <is>
@@ -24954,7 +24954,7 @@
         <v>2</v>
       </c>
       <c r="I572">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J572" t="inlineStr">
         <is>
@@ -24997,7 +24997,7 @@
         <v>2</v>
       </c>
       <c r="I573">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J573" t="inlineStr">
         <is>
@@ -25040,7 +25040,7 @@
         <v>2</v>
       </c>
       <c r="I574">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J574" t="inlineStr">
         <is>
@@ -25083,7 +25083,7 @@
         <v>2</v>
       </c>
       <c r="I575">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J575" t="inlineStr">
         <is>
@@ -25126,7 +25126,7 @@
         <v>2</v>
       </c>
       <c r="I576">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J576" t="inlineStr">
         <is>
@@ -25169,7 +25169,7 @@
         <v>2</v>
       </c>
       <c r="I577">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J577" t="inlineStr">
         <is>
@@ -25212,7 +25212,7 @@
         <v>2</v>
       </c>
       <c r="I578">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J578" t="inlineStr">
         <is>
@@ -25255,7 +25255,7 @@
         <v>2</v>
       </c>
       <c r="I579">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J579" t="inlineStr">
         <is>
@@ -25298,7 +25298,7 @@
         <v>2</v>
       </c>
       <c r="I580">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J580" t="inlineStr">
         <is>
@@ -25341,7 +25341,7 @@
         <v>2</v>
       </c>
       <c r="I581">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J581" t="inlineStr">
         <is>
@@ -25384,7 +25384,7 @@
         <v>2</v>
       </c>
       <c r="I582">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J582" t="inlineStr">
         <is>
@@ -25427,7 +25427,7 @@
         <v>2</v>
       </c>
       <c r="I583">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J583" t="inlineStr">
         <is>
@@ -25470,7 +25470,7 @@
         <v>2</v>
       </c>
       <c r="I584">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J584" t="inlineStr">
         <is>
@@ -28475,7 +28475,7 @@
         <v>3383</v>
       </c>
       <c r="G654">
-        <v>0.68</v>
+        <v>0.6800000000000001</v>
       </c>
       <c r="H654">
         <v>1</v>
@@ -28518,7 +28518,7 @@
         <v>2422</v>
       </c>
       <c r="G655">
-        <v>0.68</v>
+        <v>0.6800000000000001</v>
       </c>
       <c r="H655">
         <v>1</v>
@@ -28561,7 +28561,7 @@
         <v>22704</v>
       </c>
       <c r="G656">
-        <v>0.6899999999999999</v>
+        <v>0.69</v>
       </c>
       <c r="H656">
         <v>1</v>
@@ -28604,7 +28604,7 @@
         <v>13102</v>
       </c>
       <c r="G657">
-        <v>0.6899999999999999</v>
+        <v>0.69</v>
       </c>
       <c r="H657">
         <v>1</v>
@@ -28647,7 +28647,7 @@
         <v>6609</v>
       </c>
       <c r="G658">
-        <v>0.6899999999999999</v>
+        <v>0.69</v>
       </c>
       <c r="H658">
         <v>1</v>
@@ -28690,7 +28690,7 @@
         <v>5281</v>
       </c>
       <c r="G659">
-        <v>0.6899999999999999</v>
+        <v>0.69</v>
       </c>
       <c r="H659">
         <v>1</v>
@@ -28733,7 +28733,7 @@
         <v>4531</v>
       </c>
       <c r="G660">
-        <v>0.6899999999999999</v>
+        <v>0.69</v>
       </c>
       <c r="H660">
         <v>1</v>
@@ -28776,7 +28776,7 @@
         <v>3521</v>
       </c>
       <c r="G661">
-        <v>0.6899999999999999</v>
+        <v>0.69</v>
       </c>
       <c r="H661">
         <v>1</v>
@@ -28819,7 +28819,7 @@
         <v>3225</v>
       </c>
       <c r="G662">
-        <v>0.6899999999999999</v>
+        <v>0.69</v>
       </c>
       <c r="H662">
         <v>1</v>
@@ -28862,7 +28862,7 @@
         <v>2371</v>
       </c>
       <c r="G663">
-        <v>0.6899999999999999</v>
+        <v>0.69</v>
       </c>
       <c r="H663">
         <v>1</v>
@@ -30427,1021 +30427,6 @@
         <is>
           <t>LOW</t>
         </is>
-      </c>
-    </row>
-    <row r="700">
-      <c r="A700" t="inlineStr">
-        <is>
-          <t>Uttarakhand</t>
-        </is>
-      </c>
-      <c r="B700" t="inlineStr">
-        <is>
-          <t>Dehradun</t>
-        </is>
-      </c>
-      <c r="C700">
-        <v>727</v>
-      </c>
-      <c r="D700">
-        <v>810</v>
-      </c>
-      <c r="E700">
-        <v>969</v>
-      </c>
-      <c r="F700">
-        <v>33533</v>
-      </c>
-      <c r="G700">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="701">
-      <c r="A701" t="inlineStr">
-        <is>
-          <t>Karnataka</t>
-        </is>
-      </c>
-      <c r="B701" t="inlineStr">
-        <is>
-          <t>Udupi</t>
-        </is>
-      </c>
-      <c r="C701">
-        <v>522</v>
-      </c>
-      <c r="D701">
-        <v>571</v>
-      </c>
-      <c r="E701">
-        <v>694</v>
-      </c>
-      <c r="F701">
-        <v>14957</v>
-      </c>
-      <c r="G701">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="702">
-      <c r="A702" t="inlineStr">
-        <is>
-          <t>Karnataka</t>
-        </is>
-      </c>
-      <c r="B702" t="inlineStr">
-        <is>
-          <t>Chikkamagaluru</t>
-        </is>
-      </c>
-      <c r="C702">
-        <v>484</v>
-      </c>
-      <c r="D702">
-        <v>529</v>
-      </c>
-      <c r="E702">
-        <v>647</v>
-      </c>
-      <c r="F702">
-        <v>4523</v>
-      </c>
-      <c r="G702">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="703">
-      <c r="A703" t="inlineStr">
-        <is>
-          <t>Assam</t>
-        </is>
-      </c>
-      <c r="B703" t="inlineStr">
-        <is>
-          <t>Sonitpur</t>
-        </is>
-      </c>
-      <c r="C703">
-        <v>649</v>
-      </c>
-      <c r="D703">
-        <v>723</v>
-      </c>
-      <c r="E703">
-        <v>862</v>
-      </c>
-      <c r="F703">
-        <v>4019</v>
-      </c>
-      <c r="G703">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="704">
-      <c r="A704" t="inlineStr">
-        <is>
-          <t>Sikkim</t>
-        </is>
-      </c>
-      <c r="B704" t="inlineStr">
-        <is>
-          <t>East District</t>
-        </is>
-      </c>
-      <c r="C704">
-        <v>546</v>
-      </c>
-      <c r="D704">
-        <v>587</v>
-      </c>
-      <c r="E704">
-        <v>724</v>
-      </c>
-      <c r="F704">
-        <v>3879</v>
-      </c>
-      <c r="G704">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="705">
-      <c r="A705" t="inlineStr">
-        <is>
-          <t>Maharashtra</t>
-        </is>
-      </c>
-      <c r="B705" t="inlineStr">
-        <is>
-          <t>Pune</t>
-        </is>
-      </c>
-      <c r="C705">
-        <v>576</v>
-      </c>
-      <c r="D705">
-        <v>662</v>
-      </c>
-      <c r="E705">
-        <v>757</v>
-      </c>
-      <c r="F705">
-        <v>45463</v>
-      </c>
-      <c r="G705">
-        <v>0.76</v>
-      </c>
-    </row>
-    <row r="706">
-      <c r="A706" t="inlineStr">
-        <is>
-          <t>Kerala</t>
-        </is>
-      </c>
-      <c r="B706" t="inlineStr">
-        <is>
-          <t>Idukki</t>
-        </is>
-      </c>
-      <c r="C706">
-        <v>482</v>
-      </c>
-      <c r="D706">
-        <v>526</v>
-      </c>
-      <c r="E706">
-        <v>637</v>
-      </c>
-      <c r="F706">
-        <v>23385</v>
-      </c>
-      <c r="G706">
-        <v>0.76</v>
-      </c>
-    </row>
-    <row r="707">
-      <c r="A707" t="inlineStr">
-        <is>
-          <t>Tamil Nadu</t>
-        </is>
-      </c>
-      <c r="B707" t="inlineStr">
-        <is>
-          <t>Tiruppur</t>
-        </is>
-      </c>
-      <c r="C707">
-        <v>480</v>
-      </c>
-      <c r="D707">
-        <v>520</v>
-      </c>
-      <c r="E707">
-        <v>630</v>
-      </c>
-      <c r="F707">
-        <v>14078</v>
-      </c>
-      <c r="G707">
-        <v>0.76</v>
-      </c>
-    </row>
-    <row r="708">
-      <c r="A708" t="inlineStr">
-        <is>
-          <t>Assam</t>
-        </is>
-      </c>
-      <c r="B708" t="inlineStr">
-        <is>
-          <t>Golaghat</t>
-        </is>
-      </c>
-      <c r="C708">
-        <v>670</v>
-      </c>
-      <c r="D708">
-        <v>775</v>
-      </c>
-      <c r="E708">
-        <v>880</v>
-      </c>
-      <c r="F708">
-        <v>4253</v>
-      </c>
-      <c r="G708">
-        <v>0.76</v>
-      </c>
-    </row>
-    <row r="709">
-      <c r="A709" t="inlineStr">
-        <is>
-          <t>Kerala</t>
-        </is>
-      </c>
-      <c r="B709" t="inlineStr">
-        <is>
-          <t>Ernakulam</t>
-        </is>
-      </c>
-      <c r="C709">
-        <v>561</v>
-      </c>
-      <c r="D709">
-        <v>642</v>
-      </c>
-      <c r="E709">
-        <v>732</v>
-      </c>
-      <c r="F709">
-        <v>63647</v>
-      </c>
-      <c r="G709">
-        <v>0.77</v>
-      </c>
-    </row>
-    <row r="710">
-      <c r="A710" t="inlineStr">
-        <is>
-          <t>Tamil Nadu</t>
-        </is>
-      </c>
-      <c r="B710" t="inlineStr">
-        <is>
-          <t>Chennai</t>
-        </is>
-      </c>
-      <c r="C710">
-        <v>476</v>
-      </c>
-      <c r="D710">
-        <v>554</v>
-      </c>
-      <c r="E710">
-        <v>616</v>
-      </c>
-      <c r="F710">
-        <v>35492</v>
-      </c>
-      <c r="G710">
-        <v>0.77</v>
-      </c>
-    </row>
-    <row r="711">
-      <c r="A711" t="inlineStr">
-        <is>
-          <t>Kerala</t>
-        </is>
-      </c>
-      <c r="B711" t="inlineStr">
-        <is>
-          <t>Malappuram</t>
-        </is>
-      </c>
-      <c r="C711">
-        <v>532</v>
-      </c>
-      <c r="D711">
-        <v>564</v>
-      </c>
-      <c r="E711">
-        <v>693</v>
-      </c>
-      <c r="F711">
-        <v>16492</v>
-      </c>
-      <c r="G711">
-        <v>0.77</v>
-      </c>
-    </row>
-    <row r="712">
-      <c r="A712" t="inlineStr">
-        <is>
-          <t>Gujarat</t>
-        </is>
-      </c>
-      <c r="B712" t="inlineStr">
-        <is>
-          <t>Kachchh</t>
-        </is>
-      </c>
-      <c r="C712">
-        <v>550</v>
-      </c>
-      <c r="D712">
-        <v>581</v>
-      </c>
-      <c r="E712">
-        <v>712</v>
-      </c>
-      <c r="F712">
-        <v>14410</v>
-      </c>
-      <c r="G712">
-        <v>0.77</v>
-      </c>
-    </row>
-    <row r="713">
-      <c r="A713" t="inlineStr">
-        <is>
-          <t>Karnataka</t>
-        </is>
-      </c>
-      <c r="B713" t="inlineStr">
-        <is>
-          <t>Dakshina Kannada</t>
-        </is>
-      </c>
-      <c r="C713">
-        <v>520</v>
-      </c>
-      <c r="D713">
-        <v>548</v>
-      </c>
-      <c r="E713">
-        <v>671</v>
-      </c>
-      <c r="F713">
-        <v>11681</v>
-      </c>
-      <c r="G713">
-        <v>0.77</v>
-      </c>
-    </row>
-    <row r="714">
-      <c r="A714" t="inlineStr">
-        <is>
-          <t>Arunachal Pradesh</t>
-        </is>
-      </c>
-      <c r="B714" t="inlineStr">
-        <is>
-          <t>Changlang</t>
-        </is>
-      </c>
-      <c r="C714">
-        <v>600</v>
-      </c>
-      <c r="D714">
-        <v>727</v>
-      </c>
-      <c r="E714">
-        <v>784</v>
-      </c>
-      <c r="F714">
-        <v>2393</v>
-      </c>
-      <c r="G714">
-        <v>0.77</v>
-      </c>
-    </row>
-    <row r="715">
-      <c r="A715" t="inlineStr">
-        <is>
-          <t>Karnataka</t>
-        </is>
-      </c>
-      <c r="B715" t="inlineStr">
-        <is>
-          <t>Bangalore</t>
-        </is>
-      </c>
-      <c r="C715">
-        <v>527</v>
-      </c>
-      <c r="D715">
-        <v>575</v>
-      </c>
-      <c r="E715">
-        <v>677</v>
-      </c>
-      <c r="F715">
-        <v>112172</v>
-      </c>
-      <c r="G715">
-        <v>0.78</v>
-      </c>
-    </row>
-    <row r="716">
-      <c r="A716" t="inlineStr">
-        <is>
-          <t>Kerala</t>
-        </is>
-      </c>
-      <c r="B716" t="inlineStr">
-        <is>
-          <t>Palakkad</t>
-        </is>
-      </c>
-      <c r="C716">
-        <v>554</v>
-      </c>
-      <c r="D716">
-        <v>589</v>
-      </c>
-      <c r="E716">
-        <v>706</v>
-      </c>
-      <c r="F716">
-        <v>35876</v>
-      </c>
-      <c r="G716">
-        <v>0.78</v>
-      </c>
-    </row>
-    <row r="717">
-      <c r="A717" t="inlineStr">
-        <is>
-          <t>Uttarakhand</t>
-        </is>
-      </c>
-      <c r="B717" t="inlineStr">
-        <is>
-          <t>Nainital</t>
-        </is>
-      </c>
-      <c r="C717">
-        <v>771</v>
-      </c>
-      <c r="D717">
-        <v>865</v>
-      </c>
-      <c r="E717">
-        <v>987</v>
-      </c>
-      <c r="F717">
-        <v>26390</v>
-      </c>
-      <c r="G717">
-        <v>0.78</v>
-      </c>
-    </row>
-    <row r="718">
-      <c r="A718" t="inlineStr">
-        <is>
-          <t>Ladakh</t>
-        </is>
-      </c>
-      <c r="B718" t="inlineStr">
-        <is>
-          <t>Leh</t>
-        </is>
-      </c>
-      <c r="C718">
-        <v>531</v>
-      </c>
-      <c r="D718">
-        <v>586</v>
-      </c>
-      <c r="E718">
-        <v>682</v>
-      </c>
-      <c r="F718">
-        <v>12575</v>
-      </c>
-      <c r="G718">
-        <v>0.78</v>
-      </c>
-    </row>
-    <row r="719">
-      <c r="A719" t="inlineStr">
-        <is>
-          <t>Goa</t>
-        </is>
-      </c>
-      <c r="B719" t="inlineStr">
-        <is>
-          <t>South Goa</t>
-        </is>
-      </c>
-      <c r="C719">
-        <v>537</v>
-      </c>
-      <c r="D719">
-        <v>565</v>
-      </c>
-      <c r="E719">
-        <v>691</v>
-      </c>
-      <c r="F719">
-        <v>11385</v>
-      </c>
-      <c r="G719">
-        <v>0.78</v>
-      </c>
-    </row>
-    <row r="720">
-      <c r="A720" t="inlineStr">
-        <is>
-          <t>Chhattisgarh</t>
-        </is>
-      </c>
-      <c r="B720" t="inlineStr">
-        <is>
-          <t>Raigad</t>
-        </is>
-      </c>
-      <c r="C720">
-        <v>572</v>
-      </c>
-      <c r="D720">
-        <v>607</v>
-      </c>
-      <c r="E720">
-        <v>737</v>
-      </c>
-      <c r="F720">
-        <v>11257</v>
-      </c>
-      <c r="G720">
-        <v>0.78</v>
-      </c>
-    </row>
-    <row r="721">
-      <c r="A721" t="inlineStr">
-        <is>
-          <t>Maharashtra</t>
-        </is>
-      </c>
-      <c r="B721" t="inlineStr">
-        <is>
-          <t>Raigad</t>
-        </is>
-      </c>
-      <c r="C721">
-        <v>572</v>
-      </c>
-      <c r="D721">
-        <v>607</v>
-      </c>
-      <c r="E721">
-        <v>737</v>
-      </c>
-      <c r="F721">
-        <v>11257</v>
-      </c>
-      <c r="G721">
-        <v>0.78</v>
-      </c>
-    </row>
-    <row r="722">
-      <c r="A722" t="inlineStr">
-        <is>
-          <t>Assam</t>
-        </is>
-      </c>
-      <c r="B722" t="inlineStr">
-        <is>
-          <t>Tinsukia</t>
-        </is>
-      </c>
-      <c r="C722">
-        <v>693</v>
-      </c>
-      <c r="D722">
-        <v>755</v>
-      </c>
-      <c r="E722">
-        <v>888</v>
-      </c>
-      <c r="F722">
-        <v>5848</v>
-      </c>
-      <c r="G722">
-        <v>0.78</v>
-      </c>
-    </row>
-    <row r="723">
-      <c r="A723" t="inlineStr">
-        <is>
-          <t>Goa</t>
-        </is>
-      </c>
-      <c r="B723" t="inlineStr">
-        <is>
-          <t>North Goa</t>
-        </is>
-      </c>
-      <c r="C723">
-        <v>572</v>
-      </c>
-      <c r="D723">
-        <v>629</v>
-      </c>
-      <c r="E723">
-        <v>723</v>
-      </c>
-      <c r="F723">
-        <v>16767</v>
-      </c>
-      <c r="G723">
-        <v>0.79</v>
-      </c>
-    </row>
-    <row r="724">
-      <c r="A724" t="inlineStr">
-        <is>
-          <t>Kerala</t>
-        </is>
-      </c>
-      <c r="B724" t="inlineStr">
-        <is>
-          <t>Thrissur</t>
-        </is>
-      </c>
-      <c r="C724">
-        <v>579</v>
-      </c>
-      <c r="D724">
-        <v>624</v>
-      </c>
-      <c r="E724">
-        <v>723</v>
-      </c>
-      <c r="F724">
-        <v>41673</v>
-      </c>
-      <c r="G724">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="725">
-      <c r="A725" t="inlineStr">
-        <is>
-          <t>Karnataka</t>
-        </is>
-      </c>
-      <c r="B725" t="inlineStr">
-        <is>
-          <t>Uttara Kannada</t>
-        </is>
-      </c>
-      <c r="C725">
-        <v>563</v>
-      </c>
-      <c r="D725">
-        <v>596</v>
-      </c>
-      <c r="E725">
-        <v>707</v>
-      </c>
-      <c r="F725">
-        <v>11080</v>
-      </c>
-      <c r="G725">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="726">
-      <c r="A726" t="inlineStr">
-        <is>
-          <t>Arunachal Pradesh</t>
-        </is>
-      </c>
-      <c r="B726" t="inlineStr">
-        <is>
-          <t>West Kameng</t>
-        </is>
-      </c>
-      <c r="C726">
-        <v>654</v>
-      </c>
-      <c r="D726">
-        <v>737</v>
-      </c>
-      <c r="E726">
-        <v>819</v>
-      </c>
-      <c r="F726">
-        <v>10467</v>
-      </c>
-      <c r="G726">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="727">
-      <c r="A727" t="inlineStr">
-        <is>
-          <t>Rajasthan</t>
-        </is>
-      </c>
-      <c r="B727" t="inlineStr">
-        <is>
-          <t>Jaisalmer</t>
-        </is>
-      </c>
-      <c r="C727">
-        <v>424</v>
-      </c>
-      <c r="D727">
-        <v>457</v>
-      </c>
-      <c r="E727">
-        <v>530</v>
-      </c>
-      <c r="F727">
-        <v>4397</v>
-      </c>
-      <c r="G727">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="728">
-      <c r="A728" t="inlineStr">
-        <is>
-          <t>Kerala</t>
-        </is>
-      </c>
-      <c r="B728" t="inlineStr">
-        <is>
-          <t>Kannur</t>
-        </is>
-      </c>
-      <c r="C728">
-        <v>594</v>
-      </c>
-      <c r="D728">
-        <v>647</v>
-      </c>
-      <c r="E728">
-        <v>735</v>
-      </c>
-      <c r="F728">
-        <v>28964</v>
-      </c>
-      <c r="G728">
-        <v>0.8100000000000001</v>
-      </c>
-    </row>
-    <row r="729">
-      <c r="A729" t="inlineStr">
-        <is>
-          <t>Karnataka</t>
-        </is>
-      </c>
-      <c r="B729" t="inlineStr">
-        <is>
-          <t>Chamarajanagara</t>
-        </is>
-      </c>
-      <c r="C729">
-        <v>525</v>
-      </c>
-      <c r="D729">
-        <v>561</v>
-      </c>
-      <c r="E729">
-        <v>650</v>
-      </c>
-      <c r="F729">
-        <v>6425</v>
-      </c>
-      <c r="G729">
-        <v>0.8100000000000001</v>
-      </c>
-    </row>
-    <row r="730">
-      <c r="A730" t="inlineStr">
-        <is>
-          <t>West Bengal</t>
-        </is>
-      </c>
-      <c r="B730" t="inlineStr">
-        <is>
-          <t>Darjeeling</t>
-        </is>
-      </c>
-      <c r="C730">
-        <v>751</v>
-      </c>
-      <c r="D730">
-        <v>808</v>
-      </c>
-      <c r="E730">
-        <v>917</v>
-      </c>
-      <c r="F730">
-        <v>7903</v>
-      </c>
-      <c r="G730">
-        <v>0.82</v>
-      </c>
-    </row>
-    <row r="731">
-      <c r="A731" t="inlineStr">
-        <is>
-          <t>Karnataka</t>
-        </is>
-      </c>
-      <c r="B731" t="inlineStr">
-        <is>
-          <t>Mysuru</t>
-        </is>
-      </c>
-      <c r="C731">
-        <v>563</v>
-      </c>
-      <c r="D731">
-        <v>607</v>
-      </c>
-      <c r="E731">
-        <v>673</v>
-      </c>
-      <c r="F731">
-        <v>36355</v>
-      </c>
-      <c r="G731">
-        <v>0.84</v>
-      </c>
-    </row>
-    <row r="732">
-      <c r="A732" t="inlineStr">
-        <is>
-          <t>Arunachal Pradesh</t>
-        </is>
-      </c>
-      <c r="B732" t="inlineStr">
-        <is>
-          <t>Lower Dibang Valley</t>
-        </is>
-      </c>
-      <c r="C732">
-        <v>689</v>
-      </c>
-      <c r="D732">
-        <v>808</v>
-      </c>
-      <c r="E732">
-        <v>825</v>
-      </c>
-      <c r="F732">
-        <v>4606</v>
-      </c>
-      <c r="G732">
-        <v>0.84</v>
-      </c>
-    </row>
-    <row r="733">
-      <c r="A733" t="inlineStr">
-        <is>
-          <t>Tamil Nadu</t>
-        </is>
-      </c>
-      <c r="B733" t="inlineStr">
-        <is>
-          <t>Coimbatore</t>
-        </is>
-      </c>
-      <c r="C733">
-        <v>583</v>
-      </c>
-      <c r="D733">
-        <v>605</v>
-      </c>
-      <c r="E733">
-        <v>672</v>
-      </c>
-      <c r="F733">
-        <v>52089</v>
-      </c>
-      <c r="G733">
-        <v>0.87</v>
-      </c>
-    </row>
-    <row r="734">
-      <c r="A734" t="inlineStr">
-        <is>
-          <t>Andaman and Nicobar Islands</t>
-        </is>
-      </c>
-      <c r="B734" t="inlineStr">
-        <is>
-          <t>Nicobar</t>
-        </is>
-      </c>
-      <c r="C734">
-        <v>219</v>
-      </c>
-      <c r="D734">
-        <v>276</v>
-      </c>
-      <c r="E734">
-        <v>242</v>
-      </c>
-      <c r="F734">
-        <v>1535</v>
-      </c>
-      <c r="G734">
-        <v>0.9</v>
-      </c>
-    </row>
-    <row r="735">
-      <c r="A735" t="inlineStr">
-        <is>
-          <t>Andaman and Nicobar Islands</t>
-        </is>
-      </c>
-      <c r="B735" t="inlineStr">
-        <is>
-          <t>South Andaman</t>
-        </is>
-      </c>
-      <c r="C735">
-        <v>370</v>
-      </c>
-      <c r="D735">
-        <v>414</v>
-      </c>
-      <c r="E735">
-        <v>387</v>
-      </c>
-      <c r="F735">
-        <v>11563</v>
-      </c>
-      <c r="G735">
-        <v>0.96</v>
-      </c>
-    </row>
-    <row r="736">
-      <c r="A736" t="inlineStr">
-        <is>
-          <t>Lakshadweep</t>
-        </is>
-      </c>
-      <c r="B736" t="inlineStr">
-        <is>
-          <t>Lakshadweep</t>
-        </is>
-      </c>
-      <c r="C736">
-        <v>139</v>
-      </c>
-      <c r="D736">
-        <v>194</v>
-      </c>
-      <c r="E736">
-        <v>140</v>
-      </c>
-      <c r="F736">
-        <v>313</v>
-      </c>
-      <c r="G736">
-        <v>0.99</v>
-      </c>
-    </row>
-    <row r="737">
-      <c r="B737" t="inlineStr">
-        <is>
-          <t>Dadra &amp; Nagar Haveli</t>
-        </is>
-      </c>
-      <c r="C737">
-        <v>20</v>
-      </c>
-      <c r="D737">
-        <v>24</v>
-      </c>
-      <c r="F737">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>